<commit_message>
Signed-off-by: Srikanth Atiguppe <Srikanth.Atiguppe@languageloop.com.au>
</commit_message>
<xml_diff>
--- a/test/data/Bulk_Upload_Bookings.xlsx
+++ b/test/data/Bulk_Upload_Bookings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\har\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\ll-ui-test-automation\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1276,44 +1276,44 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" customWidth="1"/>
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="48" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="27.42578125" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="21" width="28.85546875" customWidth="1"/>
-    <col min="22" max="22" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="32.7265625" customWidth="1"/>
+    <col min="11" max="11" width="16.453125" style="48" customWidth="1"/>
+    <col min="12" max="12" width="23.54296875" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" customWidth="1"/>
+    <col min="14" max="14" width="23.1796875" customWidth="1"/>
+    <col min="15" max="15" width="29.26953125" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" customWidth="1"/>
+    <col min="17" max="17" width="27.453125" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" customWidth="1"/>
+    <col min="19" max="19" width="11.1796875" customWidth="1"/>
+    <col min="20" max="20" width="14.26953125" customWidth="1"/>
+    <col min="21" max="21" width="28.81640625" customWidth="1"/>
+    <col min="22" max="22" width="27.26953125" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" customWidth="1"/>
-    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31.85546875" customWidth="1"/>
-    <col min="28" max="28" width="31.85546875" style="4" customWidth="1"/>
-    <col min="29" max="29" width="32.28515625" customWidth="1"/>
-    <col min="30" max="30" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.26953125" customWidth="1"/>
+    <col min="25" max="25" width="6.81640625" customWidth="1"/>
+    <col min="26" max="26" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.81640625" customWidth="1"/>
+    <col min="28" max="28" width="31.81640625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="32.26953125" customWidth="1"/>
+    <col min="30" max="30" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
@@ -1405,12 +1405,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="36">
-        <v>44470</v>
+        <v>44835</v>
       </c>
       <c r="C2" s="37">
         <v>0.375</v>
@@ -1462,12 +1462,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="36">
-        <v>44505</v>
+        <v>44870</v>
       </c>
       <c r="C3" s="37">
         <v>0.4375</v>
@@ -1531,12 +1531,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="36">
-        <v>44506</v>
+        <v>44871</v>
       </c>
       <c r="C4" s="37">
         <v>0.46875</v>
@@ -1597,7 +1597,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28"/>
       <c r="B5" s="29"/>
       <c r="C5" s="30"/>
@@ -1628,7 +1628,7 @@
       <c r="AB5" s="31"/>
       <c r="AC5" s="22"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" s="22"/>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
@@ -1659,7 +1659,7 @@
       <c r="AB6" s="22"/>
       <c r="AC6" s="22"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="22"/>
       <c r="B7" s="33"/>
       <c r="C7" s="34"/>
@@ -1690,7 +1690,7 @@
       <c r="AB7" s="22"/>
       <c r="AC7" s="22"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="22"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34"/>
@@ -1721,7 +1721,7 @@
       <c r="AB8" s="22"/>
       <c r="AC8" s="22"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="22"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34"/>
@@ -1752,7 +1752,7 @@
       <c r="AB9" s="22"/>
       <c r="AC9" s="22"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="33"/>
       <c r="C10" s="34"/>
@@ -1783,7 +1783,7 @@
       <c r="AB10" s="22"/>
       <c r="AC10" s="22"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="33"/>
       <c r="C11" s="34"/>
@@ -1814,7 +1814,7 @@
       <c r="AB11" s="22"/>
       <c r="AC11" s="22"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="22"/>
       <c r="B12" s="33"/>
       <c r="C12" s="34"/>
@@ -1845,7 +1845,7 @@
       <c r="AB12" s="22"/>
       <c r="AC12" s="22"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="22"/>
       <c r="B13" s="33"/>
       <c r="C13" s="34"/>
@@ -1876,7 +1876,7 @@
       <c r="AB13" s="22"/>
       <c r="AC13" s="22"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="22"/>
       <c r="B14" s="33"/>
       <c r="C14" s="34"/>
@@ -1907,7 +1907,7 @@
       <c r="AB14" s="22"/>
       <c r="AC14" s="22"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="22"/>
       <c r="B15" s="33"/>
       <c r="C15" s="34"/>
@@ -1938,7 +1938,7 @@
       <c r="AB15" s="22"/>
       <c r="AC15" s="22"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="22"/>
       <c r="B16" s="33"/>
       <c r="C16" s="34"/>
@@ -1990,19 +1990,19 @@
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="12" customWidth="1"/>
     <col min="6" max="6" width="3" style="4" customWidth="1"/>
-    <col min="7" max="7" width="56.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="4"/>
+    <col min="7" max="7" width="56.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="G1" s="18"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>43476</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="E23" s="13"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>2</v>
       </c>
@@ -2394,7 +2394,7 @@
       </c>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="G25" s="20"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Fix Bulk Upload Booking Interview Date data
</commit_message>
<xml_diff>
--- a/test/data/Bulk_Upload_Bookings.xlsx
+++ b/test/data/Bulk_Upload_Bookings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\ll-ui-test-automation\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohammed.ubeduddin\Documents\LanguageLoop\Repo\ll-ui-test-automation\premaster\ll-ui-test-automation\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1410,7 +1410,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="36">
-        <v>44835</v>
+        <v>45566</v>
       </c>
       <c r="C2" s="37">
         <v>0.375</v>
@@ -1467,7 +1467,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="36">
-        <v>44870</v>
+        <v>45601</v>
       </c>
       <c r="C3" s="37">
         <v>0.4375</v>
@@ -1536,7 +1536,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="36">
-        <v>44871</v>
+        <v>45602</v>
       </c>
       <c r="C4" s="37">
         <v>0.46875</v>

</xml_diff>

<commit_message>
Fixed data in Bulk upload booking file
</commit_message>
<xml_diff>
--- a/test/data/Bulk_Upload_Bookings.xlsx
+++ b/test/data/Bulk_Upload_Bookings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
   <si>
     <t>Job Notes</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>wh@wh.org</t>
-  </si>
-  <si>
-    <t>1 Aquatic Drive</t>
   </si>
   <si>
     <t>Maribyrnong</t>
@@ -1275,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1402,7 +1399,7 @@
         <v>48</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.35">
@@ -1430,7 +1427,7 @@
         <v>54</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L2" s="45" t="s">
         <v>73</v>
@@ -1459,7 +1456,7 @@
       <c r="AB2" s="39"/>
       <c r="AC2" s="39"/>
       <c r="AD2" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.35">
@@ -1490,7 +1487,7 @@
         <v>60</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L3" s="39"/>
       <c r="M3" s="40"/>
@@ -1507,28 +1504,20 @@
         <v>72</v>
       </c>
       <c r="T3" s="39"/>
-      <c r="U3" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="W3" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="X3" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y3" s="39" t="s">
-        <v>77</v>
-      </c>
+      <c r="U3" s="38"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
       <c r="Z3" s="39"/>
       <c r="AA3" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB3" s="39"/>
       <c r="AC3" s="42" t="s">
         <v>61</v>
       </c>
       <c r="AD3" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.35">
@@ -1557,7 +1546,7 @@
       </c>
       <c r="J4" s="39"/>
       <c r="K4" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L4" s="44" t="s">
         <v>66</v>
@@ -1575,17 +1564,17 @@
         <v>1</v>
       </c>
       <c r="U4" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V4" s="39"/>
       <c r="W4" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="X4" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="X4" s="39" t="s">
+      <c r="Y4" s="39" t="s">
         <v>76</v>
-      </c>
-      <c r="Y4" s="39" t="s">
-        <v>77</v>
       </c>
       <c r="Z4" s="39"/>
       <c r="AA4" s="39"/>
@@ -1594,7 +1583,7 @@
         <v>69</v>
       </c>
       <c r="AD4" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1986,7 +1975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>

</xml_diff>